<commit_message>
Add Marital Relationship Form feature
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/marital_relationship_form.xlsx
+++ b/app/src/main/res/raw/marital_relationship_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30720" windowHeight="13512" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="11925" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
   <si>
     <t>group</t>
   </si>
@@ -91,16 +91,25 @@
     <t>header</t>
   </si>
   <si>
+    <t>visitCode</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>1.0. Visit Code</t>
+  </si>
+  <si>
+    <t>1.0. Código da Visita</t>
+  </si>
+  <si>
     <t>memberA</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>1.1. Member A Code</t>
   </si>
   <si>
-    <t>1.1. Código do Membro</t>
+    <t>1.1. Código do Membro A</t>
   </si>
   <si>
     <t>memberA_name</t>
@@ -109,7 +118,7 @@
     <t>1.2. Member A Name</t>
   </si>
   <si>
-    <t>1.2. Código do Agregado</t>
+    <t>1.2. Nome do Membro A</t>
   </si>
   <si>
     <t>memberB</t>
@@ -118,7 +127,7 @@
     <t>1.3. Member B Code</t>
   </si>
   <si>
-    <t>1.3. Nome do Agregado</t>
+    <t>1.3. Código do Membro B</t>
   </si>
   <si>
     <t>memberB_name</t>
@@ -127,16 +136,22 @@
     <t>1.4. Member B Name</t>
   </si>
   <si>
-    <t>2.1. Código da Mãe</t>
-  </si>
-  <si>
-    <t>status</t>
+    <t>1.4. Nome do Membro B</t>
   </si>
   <si>
     <t>memberA_status</t>
   </si>
   <si>
-    <t>2.1 Current Marital Status of Member A</t>
+    <t>select</t>
+  </si>
+  <si>
+    <t>marital_statuses</t>
+  </si>
+  <si>
+    <t>2.1. Current Marital Status of Member A</t>
+  </si>
+  <si>
+    <t>2.1. Estado Civil do Membro A</t>
   </si>
   <si>
     <t>memberB_status</t>
@@ -145,6 +160,33 @@
     <t>2.2. Current Marital Status of Member B</t>
   </si>
   <si>
+    <t>2.2. Estado Civil do Membro B</t>
+  </si>
+  <si>
+    <t>relationshipType</t>
+  </si>
+  <si>
+    <t>marital_events</t>
+  </si>
+  <si>
+    <t>3. New Marital Status</t>
+  </si>
+  <si>
+    <t>3. Novo Estado Civil</t>
+  </si>
+  <si>
+    <t>eventDate</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>4. Event Date</t>
+  </si>
+  <si>
+    <t>4. Data do Evento</t>
+  </si>
+  <si>
     <t>collected</t>
   </si>
   <si>
@@ -154,10 +196,10 @@
     <t>username</t>
   </si>
   <si>
-    <t>4.1. Collected By Fieldworker</t>
-  </si>
-  <si>
-    <t>4.1. Códido do Inquiridor</t>
+    <t>5.1. Collected By Fieldworker</t>
+  </si>
+  <si>
+    <t>5.1. Códido do Inquiridor</t>
   </si>
   <si>
     <t>collectedDate</t>
@@ -166,10 +208,10 @@
     <t>timestamp</t>
   </si>
   <si>
-    <t>4.2. Collected Date</t>
-  </si>
-  <si>
-    <t>4.2. Data da Visita</t>
+    <t>5.2. Collected Date</t>
+  </si>
+  <si>
+    <t>5.2. Data da Visita</t>
   </si>
   <si>
     <t>value</t>
@@ -194,9 +236,6 @@
   </si>
   <si>
     <t>Feminino</t>
-  </si>
-  <si>
-    <t>relationships</t>
   </si>
   <si>
     <t>SIN</t>
@@ -276,8 +315,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -328,16 +367,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -349,6 +397,74 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
@@ -364,9 +480,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -375,82 +490,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -476,19 +515,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,157 +641,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -670,11 +709,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -684,6 +729,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -699,21 +759,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -735,15 +780,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -753,159 +789,162 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -915,7 +954,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -927,14 +966,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
@@ -1257,23 +1299,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:K16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="11.1388888888889" customWidth="true"/>
-    <col min="3" max="3" width="14.1388888888889" customWidth="true"/>
-    <col min="4" max="4" width="20.1388888888889" customWidth="true"/>
-    <col min="5" max="5" width="11.712962962963" customWidth="true"/>
-    <col min="6" max="6" width="12.287037037037" customWidth="true"/>
+    <col min="2" max="2" width="11.1428571428571" customWidth="true"/>
+    <col min="3" max="3" width="14.1428571428571" customWidth="true"/>
+    <col min="4" max="4" width="20.1428571428571" customWidth="true"/>
+    <col min="5" max="5" width="11.7142857142857" customWidth="true"/>
+    <col min="6" max="6" width="16" customWidth="true"/>
     <col min="7" max="8" width="41" customWidth="true"/>
-    <col min="9" max="9" width="21.712962962963" customWidth="true"/>
-    <col min="10" max="10" width="9.28703703703704" customWidth="true"/>
-    <col min="12" max="12" width="16.5740740740741" customWidth="true"/>
+    <col min="9" max="9" width="21.7142857142857" customWidth="true"/>
+    <col min="10" max="10" width="9.28571428571429" customWidth="true"/>
+    <col min="12" max="12" width="16.5714285714286" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1310,33 +1352,37 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
@@ -1354,7 +1400,7 @@
       <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="9"/>
+      <c r="I3" s="10"/>
       <c r="J3" t="b">
         <v>1</v>
       </c>
@@ -1378,7 +1424,7 @@
       <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="10"/>
       <c r="J4" t="b">
         <v>1</v>
       </c>
@@ -1402,7 +1448,7 @@
       <c r="H5" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="10"/>
       <c r="J5" t="b">
         <v>1</v>
       </c>
@@ -1410,123 +1456,193 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="1"/>
       <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1"/>
       <c r="D7" t="s">
         <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1"/>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="1"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="9:9">
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="9:9">
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1"/>
-      <c r="I12" s="9"/>
+      <c r="F8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1"/>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10">
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="9"/>
-      <c r="J14" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="J15" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" t="b">
-        <v>1</v>
-      </c>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17" s="1"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:1">
       <c r="A18" s="1"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:1">
       <c r="A19" s="1"/>
-      <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1"/>
@@ -1554,15 +1670,6 @@
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.39375" footer="0.39375"/>
@@ -1574,19 +1681,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="13.2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="12.5740740740741" customWidth="true"/>
-    <col min="2" max="2" width="12.287037037037" customWidth="true"/>
-    <col min="3" max="3" width="18.1388888888889" customWidth="true"/>
-    <col min="4" max="4" width="18.287037037037" customWidth="true"/>
-    <col min="5" max="5" width="13.1388888888889" customWidth="true"/>
+    <col min="1" max="1" width="19.5714285714286" customWidth="true"/>
+    <col min="2" max="2" width="12.2857142857143" customWidth="true"/>
+    <col min="3" max="3" width="18.1428571428571" customWidth="true"/>
+    <col min="4" max="4" width="18.2857142857143" customWidth="true"/>
+    <col min="5" max="5" width="13.1428571428571" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1594,7 +1701,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -1608,136 +1715,188 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>54</v>
+      <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>57</v>
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>60</v>
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>62</v>
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="D10" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="A11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="A12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1755,33 +1914,33 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="13.2" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="21.4259259259259" customWidth="true"/>
-    <col min="2" max="2" width="20.4259259259259" customWidth="true"/>
-    <col min="3" max="3" width="23.287037037037" customWidth="true"/>
+    <col min="1" max="1" width="21.4285714285714" customWidth="true"/>
+    <col min="2" max="2" width="20.4285714285714" customWidth="true"/>
+    <col min="3" max="3" width="23.2857142857143" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add Polygamic MaritalRelationship support - Fix issue not allowing Inmigration of the last individual of a Household when its the Head - Add methods to delete large database tables on SyncEntitiesTask (to avoid ObjectBox DbExceptions)
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/marital_relationship_form.xlsx
+++ b/app/src/main/res/raw/marital_relationship_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12270" tabRatio="500"/>
+    <workbookView windowWidth="27795" windowHeight="12240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="150">
   <si>
     <t>group</t>
   </si>
@@ -205,16 +205,52 @@
     <t>2.2. État civil du membre B</t>
   </si>
   <si>
+    <t>eventType</t>
+  </si>
+  <si>
+    <t>event_types</t>
+  </si>
+  <si>
+    <t>3.0.0. Marital Event Type</t>
+  </si>
+  <si>
+    <t>3.0.0. Tipo de Evento Marital</t>
+  </si>
+  <si>
+    <t>3.0.0. Type d'événement marital</t>
+  </si>
+  <si>
+    <t>isPolygamic</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>3.1. The Husband has one or more wives?</t>
+  </si>
+  <si>
+    <t>3.1. O Marido tem uma ou mais esposas?</t>
+  </si>
+  <si>
+    <t>3.1. Est-ce que le mari a une ou plusieurs femmes?</t>
+  </si>
+  <si>
+    <t>polygamicId</t>
+  </si>
+  <si>
+    <t>Polygamic Id</t>
+  </si>
+  <si>
     <t>relationshipType</t>
   </si>
   <si>
     <t>marital_events</t>
   </si>
   <si>
-    <t>3.1 New marital status</t>
-  </si>
-  <si>
-    <t>3.1. Novo Estado Civil</t>
+    <t>3.2. New marital status</t>
+  </si>
+  <si>
+    <t>3.2. Novo Estado Civil</t>
   </si>
   <si>
     <t>3.1. Nouvel état civil</t>
@@ -226,10 +262,10 @@
     <t>date</t>
   </si>
   <si>
-    <t>3.2. Event date</t>
-  </si>
-  <si>
-    <t>3.2. Data do Evento</t>
+    <t>3.3. Event date</t>
+  </si>
+  <si>
+    <t>3.3. Data do Evento</t>
   </si>
   <si>
     <t>3.2. Date de l'événement</t>
@@ -292,6 +328,24 @@
     <t>value</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
     <t>genders</t>
   </si>
   <si>
@@ -391,7 +445,37 @@
     <t>Veuf/veuve</t>
   </si>
   <si>
+    <t>START</t>
+  </si>
+  <si>
+    <t>Start Event</t>
+  </si>
+  <si>
+    <t>Início do Evento</t>
+  </si>
+  <si>
+    <t>Début de l'événement</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>End Event</t>
+  </si>
+  <si>
+    <t>Fim do Evento</t>
+  </si>
+  <si>
+    <t>Fin de l'événement</t>
+  </si>
+  <si>
+    <t>${eventType}='START'</t>
+  </si>
+  <si>
     <t>Living Together</t>
+  </si>
+  <si>
+    <t>${eventType}='END'</t>
   </si>
   <si>
     <t>form_id</t>
@@ -423,10 +507,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -447,14 +531,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -470,7 +546,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -484,8 +568,76 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -501,68 +653,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -570,27 +668,13 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
@@ -609,7 +693,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -624,55 +708,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,127 +888,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -895,11 +985,44 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -951,30 +1074,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -983,164 +1082,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1156,6 +1246,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1166,12 +1263,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1184,6 +1292,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1191,6 +1308,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1512,10 +1632,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="$A11:$XFD15"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1526,7 +1646,8 @@
     <col min="5" max="5" width="11.7238095238095" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="13.7238095238095" customWidth="1"/>
-    <col min="8" max="10" width="41" customWidth="1"/>
+    <col min="8" max="9" width="41" customWidth="1"/>
+    <col min="10" max="10" width="44.2761904761905" customWidth="1"/>
     <col min="11" max="11" width="21.7238095238095" customWidth="1"/>
     <col min="12" max="12" width="10.4571428571429" customWidth="1"/>
     <col min="13" max="13" width="9.26666666666667" customWidth="1"/>
@@ -1562,7 +1683,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="31" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1577,7 +1698,7 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="26" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -1606,8 +1727,8 @@
       <c r="J2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
       <c r="M2" t="b">
         <v>1</v>
       </c>
@@ -1634,8 +1755,8 @@
       <c r="J3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
       <c r="M3" t="b">
         <v>1</v>
       </c>
@@ -1649,15 +1770,15 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="18" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="18" t="s">
         <v>29</v>
       </c>
       <c r="I4" t="s">
@@ -1674,7 +1795,7 @@
       <c r="N4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="O4" s="18"/>
+      <c r="O4" s="26"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
@@ -1695,8 +1816,8 @@
       <c r="J5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
       <c r="M5" t="b">
         <v>1</v>
       </c>
@@ -1723,8 +1844,8 @@
       <c r="J6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
       <c r="M6" t="b">
         <v>1</v>
       </c>
@@ -1740,10 +1861,10 @@
       <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="18"/>
+      <c r="G7" s="26"/>
       <c r="H7" t="s">
         <v>43</v>
       </c>
@@ -1753,8 +1874,8 @@
       <c r="J7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
       <c r="M7" t="b">
         <v>1</v>
       </c>
@@ -1773,10 +1894,10 @@
       <c r="E8" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="18"/>
+      <c r="G8" s="26"/>
       <c r="H8" t="s">
         <v>48</v>
       </c>
@@ -1786,8 +1907,8 @@
       <c r="J8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
       <c r="M8" t="b">
         <v>1</v>
       </c>
@@ -1798,246 +1919,313 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="1"/>
-      <c r="D9" t="s">
+    <row r="9" spans="1:17">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" t="s">
+      <c r="G9" s="27"/>
+      <c r="H9" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="4:13">
-      <c r="D10" t="s">
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="N9" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" s="14" customFormat="1" spans="1:14">
+      <c r="A10" s="21"/>
+      <c r="D10" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10" s="28"/>
+      <c r="H10" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" s="11" customFormat="1" spans="1:14">
-      <c r="A11" s="15" t="s">
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="N10" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" s="14" customFormat="1" spans="1:17">
+      <c r="A11" s="22"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="I11" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1"/>
+      <c r="D12" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="11" t="s">
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="G12" s="1"/>
+      <c r="H12" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="I12" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="N11" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" s="12" customFormat="1" spans="1:14">
-      <c r="A12" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="J12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="4:13">
+      <c r="D13" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="E13" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="H13" t="s">
         <v>70</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="I13" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" s="12" customFormat="1" spans="1:17">
-      <c r="A13" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12" t="s">
+      <c r="J13" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" s="15" customFormat="1" spans="1:14">
+      <c r="A14" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12" t="s">
+      <c r="D14" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="I13" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" s="12" customFormat="1" spans="1:17">
-      <c r="A14" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12" t="s">
+      <c r="E14" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" s="16" customFormat="1" spans="1:14">
+      <c r="A15" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="N15" s="16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" s="16" customFormat="1" spans="1:17">
+      <c r="A16" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="N16" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" s="16" customFormat="1" spans="1:17">
+      <c r="A17" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" s="13" customFormat="1" spans="1:17">
-      <c r="A15" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="13" t="s">
+      <c r="H17" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="N17" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" s="17" customFormat="1" spans="1:17">
+      <c r="A18" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="1"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="1"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="1"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
+      <c r="H18" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="N18" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="1"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1"/>
@@ -2065,6 +2253,15 @@
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.39375" footer="0.39375"/>
@@ -2076,13 +2273,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G14" sqref="G14:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="19.5428571428571" customWidth="1"/>
     <col min="2" max="2" width="12.2666666666667" customWidth="1"/>
@@ -2090,14 +2287,15 @@
     <col min="4" max="4" width="20.7238095238095" customWidth="1"/>
     <col min="5" max="5" width="22.5428571428571" customWidth="1"/>
     <col min="6" max="6" width="13.1809523809524" customWidth="1"/>
+    <col min="7" max="7" width="20.6380952380952" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2111,110 +2309,117 @@
       <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="3"/>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:5">
+        <v>101</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>98</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>100</v>
-      </c>
+      <c r="B6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>104</v>
+        <v>113</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2222,16 +2427,16 @@
         <v>42</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>108</v>
+        <v>116</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2239,101 +2444,184 @@
         <v>42</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>112</v>
+        <v>121</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="7" t="s">
-        <v>52</v>
+      <c r="A10" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>96</v>
+        <v>124</v>
+      </c>
+      <c r="D10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="7" t="s">
-        <v>52</v>
+      <c r="A11" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>100</v>
+        <v>129</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>104</v>
+      <c r="B12" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="7" t="s">
-        <v>52</v>
+      <c r="B13" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G18" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2362,30 +2650,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>